<commit_message>
Add Tested Result For checkframework-dataflow
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyb19\IdeaProjects\AbuseDetection\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4312A996-D74C-44A2-A86B-A151DA972D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,26 +24,240 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+  <si>
+    <t>Tested Jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modularized?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corresponding Issue</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent reflectively method invoke: java.lang.ClassLoader.defineClass, because the project tries to reflectively invoke this method, but java.lang.ClassLoader.defineClass is protected</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cglib-3.3.0.jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>flatlaf-3.4.1.jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automatic</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Found inconsistent reflectively method invoke: sun.java2d.SunGraphicsEnvironment.isUIScaleOn, because the project tries to reflectively invoke this method, but either sun.java2d doesn't exported or opened in module declaration, or the method sun.java2d.SunGraphicsEnvironment.isUIScaleOn doesn't exist anymore in JDK 17
+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent reflectively method invoke: javax.swing.PopupFactory.getPopup, because the project tries to reflectively invoke this method, but javax.swing.PopupFactory.getPopup is protected</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent reflectively method invoke: sun.awt.shell.ShellFolder.get, because the project tries to reflectively invoke this method, but either sun.awt.shell doesn't exported or opened in module declaration, or the method sun.awt.shell.ShellFolder.get doesn't exist anymore in JDK 17</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>darklaf-core-2.6.1.jar</t>
+  </si>
+  <si>
+    <t>Found inconsistent reflectively method invoke: javax.swing.JRootPane.setUseTrueDoubleBuffering, because the project tries to reflectively invoke this method, but javax.swing.JRootPane.setUseTrueDoubleBuffering is package-private</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: sun.swing.SwingUtilities2.getSystemMnemonicKeyMask(), because the project tries to statically invoke this method, but sun.swing only exports to [jdk.unsupported.desktop]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: sun.swing.SwingUtilities2, because the project tries to statically invoke this method, but sun.swing only exports to [jdk.unsupported.desktop]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/weisJ/darklaf/issues/234</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/cglib/cglib/issues/191</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Opens" Related - Reflective Invoke</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Exports" Related - Static Invoke</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Opens" Inconsistency</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Exports"  Inconsistency</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>error_prone_check_api-2.5.1.jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent reflectively method invoke: com.sun.tools.javac.comp.Resolve.findIdent, because the project tries to reflectively invoke this method, but com.sun.tools.javac.comp only exports to [jdk.javadoc, jdk.jshell]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent reflectively method invoke: com.sun.tools.javac.util.Log.error, because the project tries to reflectively invoke this method, but either com.sun.tools.javac.util doesn't exported or opened in module declaration, or the method com.sun.tools.javac.util.Log.error doesn't exist anymore in JDK 17</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: com.sun.tools.javac.model.JavacElements, because the project tries to statically invoke this method, but com.sun.tools.javac.model only exports to [jdk.javadoc]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/google/error-prone/issues/2250</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: com.sun.tools.javac.util.JCDiagnostic$Factory, because the project tries to statically invoke this method, but com.sun.tools.javac.util only exports to [jdk.javadoc, jdk.jshell, jdk.jdeps]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: com.sun.tools.javac.util.Options, because the project tries to statically invoke this method, but com.sun.tools.javac.util only exports to [jdk.javadoc, jdk.jshell, jdk.jdeps]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: com.sun.tools.javac.util.List, because the project tries to statically invoke this method, but com.sun.tools.javac.util only exports to [jdk.javadoc, jdk.jshell, jdk.jdeps]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>msgpack-core-0.9.0.jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent reflective method invoke: java.nio.MemoryBlock.wrapFromJni, because the project tries to reflectively invoke this method, but java.nio.MemoryBlock.wrapFromJni does not exist in JDK 17</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>arthas-core-3.6.7.jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: sun.management.ManagementFactoryHelper, because the project tries to statically invoke this method, but sun.management.ManagementFactoryHelper only exports to [jdk.management, jdk.management.agent, jdk.jconsole]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/alibaba/arthas/issues/2380 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>checker-framework-dataflow-3.32.0.jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>…. 2 more</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>…. 16 more</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>…. 115 more</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>…. 4 more</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,15 +265,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +611,682 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="35.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="33.125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="24.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="33.125" customWidth="1"/>
+    <col min="8" max="8" width="54.25" customWidth="1"/>
+    <col min="9" max="9" width="16.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>18</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>117</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="29" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D33" s="2"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D34" s="2"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D35" s="2"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D36" s="2"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D37" s="2"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D38" s="2"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D39" s="2"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D40" s="2"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D41" s="2"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D42" s="2"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D43" s="2"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D44" s="2"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D45" s="2"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D46" s="2"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D47" s="2"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D49" s="2"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D50" s="2"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D51" s="2"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D52" s="2"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D53" s="2"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D54" s="2"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D55" s="2"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D56" s="2"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D57" s="2"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D58" s="2"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D59" s="2"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D60" s="2"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D61" s="2"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D62" s="2"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D63" s="2"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D64" s="2"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D65" s="2"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D66" s="2"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D67" s="2"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D68" s="2"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D69" s="2"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D70" s="2"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{E14DF816-A598-48CC-95B8-371D8374E530}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{5AF51254-139F-4FD7-BF54-4F917E35EEB7}"/>
+    <hyperlink ref="H9" r:id="rId3" xr:uid="{BE5A14DE-FDCD-4E82-9ECA-A9B9F9D409A1}"/>
+    <hyperlink ref="H13" r:id="rId4" xr:uid="{95348E82-0B02-42C6-9843-AC6D716F196B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more results & Added module info counter
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyb19\IdeaProjects\AbuseDetection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3D943A-1959-4033-B0B4-A5C502BFC5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54DB2DD-8543-49C7-A1F6-625C13401552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2115" windowWidth="38400" windowHeight="17430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="2175" windowWidth="34680" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
   <si>
     <t>Tested Jar</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -92,22 +92,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>"Opens" Related - Reflective Invoke</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Exports" Related - Static Invoke</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Opens" Inconsistency</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Exports"  Inconsistency</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>error_prone_check_api-2.5.1.jar</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -148,14 +132,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>msgpack-core-0.9.0.jar</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Found inconsistent reflective method invoke: java.nio.MemoryBlock.wrapFromJni, because the project tries to reflectively invoke this method, but java.nio.MemoryBlock.wrapFromJni does not exist in JDK 17</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>arthas-core-3.6.7.jar</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -188,6 +164,78 @@
   </si>
   <si>
     <t>darklaf-core-2.6.1.jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>google-java-format-1.22.0.jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: com.sun.tools.javac.file.BaseFileManager, because the project tries to statically invoke this method, but com.sun.tools.javac.file only exports to [jdk.javadoc, jdk.jdeps]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: com.sun.tools.javac.parser.Tokens$TokenKind, because the project tries to statically invoke this method, but com.sun.tools.javac.parser only exports to [jdk.jshell]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>…. 42 more</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/elastic/logstash/issues/13819</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>jvm-attach-api-1.5.jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent reflective method invoke: java.net.URLClassLoader.addURL, because the project tries to reflectively invoke this method, but java.net.URLClassLoader.addURL is protected</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: sun.management.counter.perf.PerfInstrumentation, because the project tries to statically invoke this method, but sun.management.counter.perf only exports to [jdk.management.agent]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: jdk.internal.perf.Perf.getPerf(), because the project tries to statically invoke this method, but jdk.internal.perf only exports to [jdk.management.agent, java.management, jdk.internal.jvmstat]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: sun.management.counter.Units, because the project tries to statically invoke this method, but sun.management.counter only exports to [jdk.management.agent]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Found inconsistent static method invoke: sun.management.counter.Variability, because the project tries to statically invoke this method, but sun.management.counter only exports to [jdk.management.agent]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>lombok-1.18.6.jar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inconsistent Exports</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inconsistent Opens</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inconsistent Exports To</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inconsistent Opens To</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reflective Invoke Inconsistency</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Static Invoke Inconsistency</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -604,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G5"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="92" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -616,14 +664,16 @@
     <col min="2" max="2" width="35.375" style="3" customWidth="1"/>
     <col min="3" max="3" width="26.375" style="3" customWidth="1"/>
     <col min="4" max="4" width="22.375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33.125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="24.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="33.125" customWidth="1"/>
-    <col min="8" max="8" width="54.25" customWidth="1"/>
-    <col min="9" max="9" width="16.125" customWidth="1"/>
+    <col min="5" max="5" width="27.625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="26.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="33.125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="24.875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="33.125" customWidth="1"/>
+    <col min="10" max="10" width="54.25" customWidth="1"/>
+    <col min="11" max="11" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -631,33 +681,39 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>16</v>
+        <v>48</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -665,37 +721,43 @@
       <c r="D2" s="3">
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="180" x14ac:dyDescent="0.2">
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C3" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="12">
         <v>0</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>4</v>
+      <c r="E3" s="12">
+        <v>44</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>4</v>
@@ -703,38 +765,45 @@
       <c r="H3" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+      <c r="I3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
-      <c r="E4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
-    </row>
-    <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.2">
+      <c r="I4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" ht="120" x14ac:dyDescent="0.2">
+      <c r="I5" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="120" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>7</v>
@@ -743,469 +812,674 @@
         <v>1</v>
       </c>
       <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12">
         <v>18</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="J6" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="7" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="J7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9" s="12">
         <v>1</v>
       </c>
       <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12">
         <v>117</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>4</v>
+      <c r="F9" s="12">
+        <v>0</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="150" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="150" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="I10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
-      <c r="G11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="I11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="135" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="12">
         <v>1</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12">
         <v>3</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="G13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+      <c r="H12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="I13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C14" s="12">
         <v>0</v>
       </c>
       <c r="D14" s="12">
+        <v>0</v>
+      </c>
+      <c r="E14" s="12">
         <v>6</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>27</v>
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+      <c r="I14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>28</v>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="I15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="G16" s="7"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" ht="180" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="12">
         <v>1</v>
       </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="D18" s="2"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="D19" s="2"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="D20" s="2"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="D21" s="2"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="D22" s="2"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23"/>
-      <c r="D23" s="2"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="D17" s="12">
+        <v>0</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="105" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" ht="150" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="12">
+        <v>1</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12">
+        <v>4</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="135" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="I21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="105" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="I22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="105" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="I23" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="105" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="12">
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0</v>
+      </c>
+      <c r="E24" s="12">
+        <v>2</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="105" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="I25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D29" s="2"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I29" s="7"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D30" s="2"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I30" s="7"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D31" s="2"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I31" s="7"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D32" s="2"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I32" s="7"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D33" s="2"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I33" s="7"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D34" s="2"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I34" s="7"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D35" s="2"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I35" s="7"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D36" s="2"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I36" s="7"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D37" s="2"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I37" s="7"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D38" s="2"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I38" s="7"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D39" s="2"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I39" s="7"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D40" s="2"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="3"/>
-    </row>
-    <row r="41" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I40" s="7"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D41" s="2"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="3"/>
-    </row>
-    <row r="42" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I41" s="7"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D42" s="2"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I42" s="7"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D43" s="2"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I43" s="7"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D44" s="2"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I44" s="7"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D45" s="2"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="3"/>
-    </row>
-    <row r="46" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I45" s="7"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D46" s="2"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I46" s="7"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D47" s="2"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="3"/>
-    </row>
-    <row r="48" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="I47" s="7"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D49" s="2"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I49" s="7"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D50" s="2"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I50" s="7"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D51" s="2"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="3"/>
-    </row>
-    <row r="52" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I51" s="7"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D52" s="2"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="3"/>
-    </row>
-    <row r="53" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I52" s="7"/>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D53" s="2"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="3"/>
-    </row>
-    <row r="54" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I53" s="7"/>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D54" s="2"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="3"/>
-    </row>
-    <row r="55" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I54" s="7"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D55" s="2"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="3"/>
-    </row>
-    <row r="56" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I55" s="7"/>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D56" s="2"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="3"/>
-    </row>
-    <row r="57" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I56" s="7"/>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D57" s="2"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="3"/>
-    </row>
-    <row r="58" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I57" s="7"/>
+      <c r="J57" s="3"/>
+    </row>
+    <row r="58" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D58" s="2"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="3"/>
-    </row>
-    <row r="59" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I58" s="7"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D59" s="2"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="3"/>
-    </row>
-    <row r="60" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I59" s="7"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D60" s="2"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="3"/>
-    </row>
-    <row r="61" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I60" s="7"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D61" s="2"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="3"/>
-    </row>
-    <row r="62" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I61" s="7"/>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D62" s="2"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="3"/>
-    </row>
-    <row r="63" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I62" s="7"/>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D63" s="2"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="3"/>
-    </row>
-    <row r="64" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I63" s="7"/>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D64" s="2"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="3"/>
-    </row>
-    <row r="65" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I64" s="7"/>
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D65" s="2"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="3"/>
-    </row>
-    <row r="66" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I65" s="7"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D66" s="2"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="3"/>
-    </row>
-    <row r="67" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I66" s="7"/>
+      <c r="J66" s="3"/>
+    </row>
+    <row r="67" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D67" s="2"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="3"/>
-    </row>
-    <row r="68" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I67" s="7"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D68" s="2"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="3"/>
-    </row>
-    <row r="69" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I68" s="7"/>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D69" s="2"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="3"/>
-    </row>
-    <row r="70" spans="4:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I69" s="7"/>
+      <c r="J69" s="3"/>
+    </row>
+    <row r="70" spans="4:10" ht="15" x14ac:dyDescent="0.2">
       <c r="D70" s="2"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="3"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="50">
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D12:D13"/>
     <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E9:E11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C6:C8"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" xr:uid="{E14DF816-A598-48CC-95B8-371D8374E530}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{5AF51254-139F-4FD7-BF54-4F917E35EEB7}"/>
-    <hyperlink ref="H9" r:id="rId3" xr:uid="{BE5A14DE-FDCD-4E82-9ECA-A9B9F9D409A1}"/>
-    <hyperlink ref="H12" r:id="rId4" xr:uid="{95348E82-0B02-42C6-9843-AC6D716F196B}"/>
+    <hyperlink ref="J6" r:id="rId1" xr:uid="{E14DF816-A598-48CC-95B8-371D8374E530}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{5AF51254-139F-4FD7-BF54-4F917E35EEB7}"/>
+    <hyperlink ref="J9" r:id="rId3" xr:uid="{BE5A14DE-FDCD-4E82-9ECA-A9B9F9D409A1}"/>
+    <hyperlink ref="J12" r:id="rId4" xr:uid="{95348E82-0B02-42C6-9843-AC6D716F196B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rename the static invocation (requires re-run the result for each subject apps)
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyb19\IdeaProjects\AbuseDetection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54DB2DD-8543-49C7-A1F6-625C13401552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B66C9B7-895A-4739-AAF8-7D6EEC9B1964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="2175" windowWidth="34680" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-840" yWindow="1470" windowWidth="34680" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -654,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="92" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:F25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="92" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1423,42 +1423,9 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A14:A15"/>
@@ -1470,9 +1437,42 @@
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C6:C8"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="D20:D23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -1480,6 +1480,7 @@
     <hyperlink ref="H2" r:id="rId2" xr:uid="{5AF51254-139F-4FD7-BF54-4F917E35EEB7}"/>
     <hyperlink ref="J9" r:id="rId3" xr:uid="{BE5A14DE-FDCD-4E82-9ECA-A9B9F9D409A1}"/>
     <hyperlink ref="J12" r:id="rId4" xr:uid="{95348E82-0B02-42C6-9843-AC6D716F196B}"/>
+    <hyperlink ref="J4" r:id="rId5" xr:uid="{F6749CE4-B267-4E90-927E-FEE594C62119}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>